<commit_message>
Actualización documentación -  Requisitos
Se realiza documento con los requisitos resultantes de las encuestas.
Se añade suposiciones y dependencias a ciclo de vida del sistema.
</commit_message>
<xml_diff>
--- a/documentos/actividades diarias.xlsx
+++ b/documentos/actividades diarias.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Fecha</t>
   </si>
@@ -53,6 +53,20 @@
     <t>1. Se crea documento de word con ciclo de vida
 2. Se añaden los pasos del estándar IEEE 830 y 1471
 3. Se añade al documento la introducción, el análisis con el problema, situación actual, objetivos, alcance, usuarios, referencias, glosario.</t>
+  </si>
+  <si>
+    <t>21/06/2016</t>
+  </si>
+  <si>
+    <t>Realización de documento funciones asesores</t>
+  </si>
+  <si>
+    <t>Análisis, Requisitos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Se crea documento de word con las funciones resultantes de las encuestas a los asesores.
+2. se crea una carpeta de requisitos, donde se iran guardando los documentos de requisitos.
+</t>
   </si>
 </sst>
 </file>
@@ -108,22 +122,22 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -142,14 +156,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B2:F10" totalsRowShown="0" headerRowDxfId="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B2:F10" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="B2:F10"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Fecha" dataDxfId="5"/>
-    <tableColumn id="2" name="Actividad" dataDxfId="4"/>
-    <tableColumn id="3" name="Fase en el ciclo de vida" dataDxfId="3"/>
-    <tableColumn id="4" name="Descripción actividad" dataDxfId="2"/>
-    <tableColumn id="5" name="Avances (%)" dataDxfId="1"/>
+    <tableColumn id="1" name="Fecha" dataDxfId="4"/>
+    <tableColumn id="2" name="Actividad" dataDxfId="3"/>
+    <tableColumn id="3" name="Fase en el ciclo de vida" dataDxfId="2"/>
+    <tableColumn id="4" name="Descripción actividad" dataDxfId="1"/>
+    <tableColumn id="5" name="Avances (%)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -421,7 +435,7 @@
   <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,11 +479,19 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+    <row r="4" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>